<commit_message>
made some changes to the simualted data excel sheet to make it easier to parse , working on making sure everything else is functional.
</commit_message>
<xml_diff>
--- a/data/Simulated_Data.xlsx
+++ b/data/Simulated_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericstine/school/CSC462/Projects/ScheduleGA4CSP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93D2129-6305-AB44-BECF-E367E517A98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE9D754-33D6-844F-9E62-17568424E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F48A5C35-C41A-416C-A9AB-2FB5F178E584}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{F48A5C35-C41A-416C-A9AB-2FB5F178E584}"/>
   </bookViews>
   <sheets>
     <sheet name="(I) Simulated Course Sections" sheetId="1" r:id="rId1"/>
@@ -60,204 +60,33 @@
     <t>MW 11:30 - 12:45pm</t>
   </si>
   <si>
-    <t>MW 1 - 2:15</t>
-  </si>
-  <si>
-    <t>MW 2:30 - 3:45</t>
-  </si>
-  <si>
-    <t>MW 4 - 5:15</t>
-  </si>
-  <si>
-    <t>MW 5:30 - 6:45</t>
-  </si>
-  <si>
-    <t>MW 7 - 8:15pm</t>
-  </si>
-  <si>
     <t>MW 8:30 - 9:45pm</t>
   </si>
   <si>
     <t>WF 11:30 - 12:45pm</t>
   </si>
   <si>
-    <t>WF 1 - 2:15</t>
-  </si>
-  <si>
-    <t>WF 2:30 - 3:45</t>
-  </si>
-  <si>
-    <t>WF 4 - 5:15</t>
-  </si>
-  <si>
-    <t>WF 5:30 - 6:45</t>
-  </si>
-  <si>
-    <t>WF 7 - 8:15pm</t>
-  </si>
-  <si>
     <t>WF 8:30 - 9:45pm</t>
   </si>
   <si>
     <t>MF 11:30 - 12:45pm</t>
   </si>
   <si>
-    <t>MF 1 - 2:15</t>
-  </si>
-  <si>
-    <t>MF 2:30 - 3:45</t>
-  </si>
-  <si>
-    <t>MF 4 - 5:15</t>
-  </si>
-  <si>
-    <t>MF 5:30 - 6:45</t>
-  </si>
-  <si>
-    <t>MF 7 - 8:15pm</t>
-  </si>
-  <si>
     <t>MF 8:30 - 9:45pm</t>
   </si>
   <si>
-    <t>MWF 7 - 7:50am</t>
-  </si>
-  <si>
-    <t>MWF 8 - 8:50am</t>
-  </si>
-  <si>
-    <t>MWF 9 - 9:50am</t>
-  </si>
-  <si>
-    <t>MWF 10 - 10:50am</t>
-  </si>
-  <si>
-    <t>MWF 11-11:50am</t>
-  </si>
-  <si>
-    <t>MWF 12 - 12:50pm</t>
-  </si>
-  <si>
-    <t>MWF 1 - 1:50pm</t>
-  </si>
-  <si>
-    <t>MWF 2 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MWF 3 - 3:50pm</t>
-  </si>
-  <si>
-    <t>MWF 4 - 4:50</t>
-  </si>
-  <si>
-    <t>MWF 5 - 5:50pm</t>
-  </si>
-  <si>
-    <t>MWF 6 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MWF 7 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MWF 8 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MWF 9 - 9:50pm</t>
-  </si>
-  <si>
-    <t>TR 7 - 8:15am</t>
-  </si>
-  <si>
     <t>TR 8:30 - 9:15am</t>
   </si>
   <si>
-    <t>TR 10 - 11:15am</t>
-  </si>
-  <si>
-    <t>TR 1 - 2:15pm</t>
-  </si>
-  <si>
     <t>TR 2:30 - 3:45pm</t>
   </si>
   <si>
-    <t>TR 4 - 5:15pm</t>
-  </si>
-  <si>
     <t>TR 5:30 - 6:45pm</t>
   </si>
   <si>
-    <t>TR 7 - 8:15pm</t>
-  </si>
-  <si>
     <t>TR 8:30 - 9:45pm</t>
   </si>
   <si>
-    <t>MW 11am - 12:50pm</t>
-  </si>
-  <si>
-    <t>MW 1 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MW 3 - 4:50pm</t>
-  </si>
-  <si>
-    <t>MW 5 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MW 6 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MW 7 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MW 8 - 9:50pm</t>
-  </si>
-  <si>
-    <t>WF 11am - 12:50pm</t>
-  </si>
-  <si>
-    <t>WF 1 - 2:50pm</t>
-  </si>
-  <si>
-    <t>WF 3 - 4:50pm</t>
-  </si>
-  <si>
-    <t>WF 5 - 6:50pm</t>
-  </si>
-  <si>
-    <t>WF 6 - 7:50pm</t>
-  </si>
-  <si>
-    <t>WF 7 - 8:50pm</t>
-  </si>
-  <si>
-    <t>WF 8 - 9:50pm</t>
-  </si>
-  <si>
-    <t>MF 11am - 12:50pm</t>
-  </si>
-  <si>
-    <t>MF 1 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MF 3 - 4:50pm</t>
-  </si>
-  <si>
-    <t>MF 5 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MF 6 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MF 7 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MF 8 - 9:50pm</t>
-  </si>
-  <si>
-    <t>MWF 7am - 8:05am</t>
-  </si>
-  <si>
     <t>MWF 8:15am - 9:20am</t>
   </si>
   <si>
@@ -267,9 +96,6 @@
     <t>MWF 10:45am - 11:50am</t>
   </si>
   <si>
-    <t>MWF 12pm - 1:05pm</t>
-  </si>
-  <si>
     <t>MWF 1:15pm - 2:20pm</t>
   </si>
   <si>
@@ -279,9 +105,6 @@
     <t>MWF 3:45pm - 4:50pm</t>
   </si>
   <si>
-    <t>MWF 5pm - 6:05pm</t>
-  </si>
-  <si>
     <t>MWF 6:15pm - 7:20pm</t>
   </si>
   <si>
@@ -291,30 +114,6 @@
     <t>MWF 8:45pm - 9:50pm</t>
   </si>
   <si>
-    <t>TR 8 - 9:50am</t>
-  </si>
-  <si>
-    <t>TR 10 - 11:50am</t>
-  </si>
-  <si>
-    <t>TR 1 - 2:50pm</t>
-  </si>
-  <si>
-    <t>TR 3 - 4:50pm</t>
-  </si>
-  <si>
-    <t>TR 5 - 6:50pm</t>
-  </si>
-  <si>
-    <t>TR 6 - 7:50pm</t>
-  </si>
-  <si>
-    <t>TR 7 - 8:50pm</t>
-  </si>
-  <si>
-    <t>TR 8 - 9:50pm</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -433,6 +232,207 @@
   </si>
   <si>
     <t>Course Number</t>
+  </si>
+  <si>
+    <t>MW 1:00 - 2:15pm</t>
+  </si>
+  <si>
+    <t>MW 2:30 - 3:45pm</t>
+  </si>
+  <si>
+    <t>MW 4:00 - 5:15pm</t>
+  </si>
+  <si>
+    <t>MW 5:30 - 6:45pm</t>
+  </si>
+  <si>
+    <t>WF 1:00 - 2:15pm</t>
+  </si>
+  <si>
+    <t>WF 2:30 - 3:45pm</t>
+  </si>
+  <si>
+    <t>WF 4:00 - 5:15pm</t>
+  </si>
+  <si>
+    <t>WF 5:30 - 6:45pm</t>
+  </si>
+  <si>
+    <t>WF 7:00 - 8:15pm</t>
+  </si>
+  <si>
+    <t>MF 1:00 - 2:15pm</t>
+  </si>
+  <si>
+    <t>MF 2:30 - 3:45pm</t>
+  </si>
+  <si>
+    <t>MF 4:00 - 5:15pm</t>
+  </si>
+  <si>
+    <t>MF 5:30 - 6:45pm</t>
+  </si>
+  <si>
+    <t>MF 7:00 - 8:15pm</t>
+  </si>
+  <si>
+    <t>MWF 7:00 - 7:50am</t>
+  </si>
+  <si>
+    <t>MWF 8:00 - 8:50am</t>
+  </si>
+  <si>
+    <t>MWF 9:00 - 9:50am</t>
+  </si>
+  <si>
+    <t>MWF 10:00 - 10:50am</t>
+  </si>
+  <si>
+    <t>MWF 11:00 - 11:50am</t>
+  </si>
+  <si>
+    <t>MWF 12:00 - 12:50pm</t>
+  </si>
+  <si>
+    <t>MWF 1:00 - 1:50pm</t>
+  </si>
+  <si>
+    <t>MWF 2:00 - 2:50pm</t>
+  </si>
+  <si>
+    <t>MWF 3:00 - 3:50pm</t>
+  </si>
+  <si>
+    <t>MWF 4:00 - 4:50pm</t>
+  </si>
+  <si>
+    <t>MWF 5:00 - 5:50pm</t>
+  </si>
+  <si>
+    <t>MWF 6:00 - 6:50pm</t>
+  </si>
+  <si>
+    <t>MWF 7:00 - 7:50pm</t>
+  </si>
+  <si>
+    <t>MWF 8:00 - 8:50pm</t>
+  </si>
+  <si>
+    <t>MWF 9:00 - 9:50pm</t>
+  </si>
+  <si>
+    <t>TR 7:00 - 8:15am</t>
+  </si>
+  <si>
+    <t>TR 10:00 - 11:15am</t>
+  </si>
+  <si>
+    <t>TR 1:00 - 2:15pm</t>
+  </si>
+  <si>
+    <t>TR 4:00 - 5:15pm</t>
+  </si>
+  <si>
+    <t>TR 7:00 - 8:15pm</t>
+  </si>
+  <si>
+    <t>MW 1:00 - 2:50pm</t>
+  </si>
+  <si>
+    <t>MW 3:00 - 4:50pm</t>
+  </si>
+  <si>
+    <t>MW 5:00 - 6:50pm</t>
+  </si>
+  <si>
+    <t>MW 6:00 - 7:50pm</t>
+  </si>
+  <si>
+    <t>MW 7:00 - 8:50pm</t>
+  </si>
+  <si>
+    <t>MW 8:00 - 9:50pm</t>
+  </si>
+  <si>
+    <t>WF 11:00am - 12:50pm</t>
+  </si>
+  <si>
+    <t>WF 1:00 - 2:50pm</t>
+  </si>
+  <si>
+    <t>WF 3:00 - 4:50pm</t>
+  </si>
+  <si>
+    <t>WF 5:00 - 6:50pm</t>
+  </si>
+  <si>
+    <t>WF 6:00 - 7:50pm</t>
+  </si>
+  <si>
+    <t>WF 7:00 - 8:50pm</t>
+  </si>
+  <si>
+    <t>WF 8:00 - 9:50pm</t>
+  </si>
+  <si>
+    <t>MF 1:00 - 2:50pm</t>
+  </si>
+  <si>
+    <t>MF 3:00 - 4:50pm</t>
+  </si>
+  <si>
+    <t>MF 5:00 - 6:50pm</t>
+  </si>
+  <si>
+    <t>MF 6:00 - 7:50pm</t>
+  </si>
+  <si>
+    <t>MF 7:00 - 8:50pm</t>
+  </si>
+  <si>
+    <t>MF 8:00 - 9:50pm</t>
+  </si>
+  <si>
+    <t>MWF 7:00am - 8:05am</t>
+  </si>
+  <si>
+    <t>MWF 12:00pm - 1:05pm</t>
+  </si>
+  <si>
+    <t>MWF 5:00pm - 6:05pm</t>
+  </si>
+  <si>
+    <t>TR 8:00 - 9:50am</t>
+  </si>
+  <si>
+    <t>TR 10:00 - 11:50am</t>
+  </si>
+  <si>
+    <t>TR 1:00 - 2:50pm</t>
+  </si>
+  <si>
+    <t>TR 3:00 - 4:50pm</t>
+  </si>
+  <si>
+    <t>TR 5:00 - 6:50pm</t>
+  </si>
+  <si>
+    <t>TR 6:00 - 7:50pm</t>
+  </si>
+  <si>
+    <t>TR 7:00 - 8:50pm</t>
+  </si>
+  <si>
+    <t>TR 8:00 - 9:50pm</t>
+  </si>
+  <si>
+    <t>MW 7:00 - 8:15pm</t>
+  </si>
+  <si>
+    <t>MW 11:00am - 12:50pm</t>
+  </si>
+  <si>
+    <t>MF 11:00am - 12:50pm</t>
   </si>
 </sst>
 </file>
@@ -819,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB0F75F-C09C-4C8D-A07D-16A4E6A47381}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -837,16 +837,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF80D7E3-E343-414F-BE36-3299F3B3A91E}">
   <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="350" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1498,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1530,7 +1530,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1538,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1546,7 +1546,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1554,7 +1554,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1562,7 +1562,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1578,7 +1578,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1586,7 +1586,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1594,7 +1594,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1602,7 +1602,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1610,7 +1610,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1618,7 +1618,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1626,7 +1626,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1634,7 +1634,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1642,7 +1642,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1650,7 +1650,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1666,7 +1666,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1674,7 +1674,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1682,7 +1682,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1690,7 +1690,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1698,7 +1698,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1706,7 +1706,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1714,7 +1714,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1722,7 +1722,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1730,7 +1730,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1738,7 +1738,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1746,7 +1746,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1754,7 +1754,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1762,7 +1762,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1770,7 +1770,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1778,7 +1778,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1786,7 +1786,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1794,7 +1794,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1802,7 +1802,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1810,7 +1810,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1842,7 +1842,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1850,7 +1850,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1858,7 +1858,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1874,7 +1874,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1882,7 +1882,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1898,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1906,7 +1906,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1914,7 +1914,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1922,7 +1922,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1930,7 +1930,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1938,7 +1938,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1946,7 +1946,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1954,7 +1954,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1970,7 +1970,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1986,7 +1986,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2018,7 +2018,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2026,7 +2026,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -2034,7 +2034,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -2042,7 +2042,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -2050,7 +2050,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -2066,7 +2066,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -2074,7 +2074,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2082,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2114,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2122,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +2130,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +2138,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +2170,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2198,25 +2198,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2494,109 +2494,109 @@
   <sheetData>
     <row r="1" spans="1:35" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
edited the simulated data and simplified some functions
</commit_message>
<xml_diff>
--- a/data/Simulated_Data.xlsx
+++ b/data/Simulated_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericstine/school/CSC462/Projects/ScheduleGA4CSP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE9D754-33D6-844F-9E62-17568424E533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAED87E-FD7E-734C-AFE0-20353683504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{F48A5C35-C41A-416C-A9AB-2FB5F178E584}"/>
   </bookViews>
@@ -57,63 +57,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>MW 11:30 - 12:45pm</t>
-  </si>
-  <si>
-    <t>MW 8:30 - 9:45pm</t>
-  </si>
-  <si>
-    <t>WF 11:30 - 12:45pm</t>
-  </si>
-  <si>
-    <t>WF 8:30 - 9:45pm</t>
-  </si>
-  <si>
-    <t>MF 11:30 - 12:45pm</t>
-  </si>
-  <si>
-    <t>MF 8:30 - 9:45pm</t>
-  </si>
-  <si>
-    <t>TR 8:30 - 9:15am</t>
-  </si>
-  <si>
-    <t>TR 2:30 - 3:45pm</t>
-  </si>
-  <si>
-    <t>TR 5:30 - 6:45pm</t>
-  </si>
-  <si>
-    <t>TR 8:30 - 9:45pm</t>
-  </si>
-  <si>
-    <t>MWF 8:15am - 9:20am</t>
-  </si>
-  <si>
-    <t>MWF 9:30am - 10:35am</t>
-  </si>
-  <si>
-    <t>MWF 10:45am - 11:50am</t>
-  </si>
-  <si>
-    <t>MWF 1:15pm - 2:20pm</t>
-  </si>
-  <si>
-    <t>MWF 2:30pm - 3:35pm</t>
-  </si>
-  <si>
-    <t>MWF 3:45pm - 4:50pm</t>
-  </si>
-  <si>
-    <t>MWF 6:15pm - 7:20pm</t>
-  </si>
-  <si>
-    <t>MWF 7:30pm - 8:35pm</t>
-  </si>
-  <si>
-    <t>MWF 8:45pm - 9:50pm</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -234,205 +177,262 @@
     <t>Course Number</t>
   </si>
   <si>
-    <t>MW 1:00 - 2:15pm</t>
-  </si>
-  <si>
-    <t>MW 2:30 - 3:45pm</t>
-  </si>
-  <si>
-    <t>MW 4:00 - 5:15pm</t>
-  </si>
-  <si>
-    <t>MW 5:30 - 6:45pm</t>
-  </si>
-  <si>
-    <t>WF 1:00 - 2:15pm</t>
-  </si>
-  <si>
-    <t>WF 2:30 - 3:45pm</t>
-  </si>
-  <si>
-    <t>WF 4:00 - 5:15pm</t>
-  </si>
-  <si>
-    <t>WF 5:30 - 6:45pm</t>
-  </si>
-  <si>
-    <t>WF 7:00 - 8:15pm</t>
-  </si>
-  <si>
-    <t>MF 1:00 - 2:15pm</t>
-  </si>
-  <si>
-    <t>MF 2:30 - 3:45pm</t>
-  </si>
-  <si>
-    <t>MF 4:00 - 5:15pm</t>
-  </si>
-  <si>
-    <t>MF 5:30 - 6:45pm</t>
-  </si>
-  <si>
-    <t>MF 7:00 - 8:15pm</t>
-  </si>
-  <si>
-    <t>MWF 7:00 - 7:50am</t>
-  </si>
-  <si>
-    <t>MWF 8:00 - 8:50am</t>
-  </si>
-  <si>
-    <t>MWF 9:00 - 9:50am</t>
-  </si>
-  <si>
-    <t>MWF 10:00 - 10:50am</t>
-  </si>
-  <si>
-    <t>MWF 11:00 - 11:50am</t>
-  </si>
-  <si>
-    <t>MWF 12:00 - 12:50pm</t>
-  </si>
-  <si>
-    <t>MWF 1:00 - 1:50pm</t>
-  </si>
-  <si>
-    <t>MWF 2:00 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MWF 3:00 - 3:50pm</t>
-  </si>
-  <si>
-    <t>MWF 4:00 - 4:50pm</t>
-  </si>
-  <si>
-    <t>MWF 5:00 - 5:50pm</t>
-  </si>
-  <si>
-    <t>MWF 6:00 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MWF 7:00 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MWF 8:00 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MWF 9:00 - 9:50pm</t>
-  </si>
-  <si>
-    <t>TR 7:00 - 8:15am</t>
-  </si>
-  <si>
-    <t>TR 10:00 - 11:15am</t>
-  </si>
-  <si>
-    <t>TR 1:00 - 2:15pm</t>
-  </si>
-  <si>
-    <t>TR 4:00 - 5:15pm</t>
-  </si>
-  <si>
-    <t>TR 7:00 - 8:15pm</t>
-  </si>
-  <si>
-    <t>MW 1:00 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MW 3:00 - 4:50pm</t>
-  </si>
-  <si>
-    <t>MW 5:00 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MW 6:00 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MW 7:00 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MW 8:00 - 9:50pm</t>
-  </si>
-  <si>
-    <t>WF 11:00am - 12:50pm</t>
-  </si>
-  <si>
-    <t>WF 1:00 - 2:50pm</t>
-  </si>
-  <si>
-    <t>WF 3:00 - 4:50pm</t>
-  </si>
-  <si>
-    <t>WF 5:00 - 6:50pm</t>
-  </si>
-  <si>
-    <t>WF 6:00 - 7:50pm</t>
-  </si>
-  <si>
-    <t>WF 7:00 - 8:50pm</t>
-  </si>
-  <si>
-    <t>WF 8:00 - 9:50pm</t>
-  </si>
-  <si>
-    <t>MF 1:00 - 2:50pm</t>
-  </si>
-  <si>
-    <t>MF 3:00 - 4:50pm</t>
-  </si>
-  <si>
-    <t>MF 5:00 - 6:50pm</t>
-  </si>
-  <si>
-    <t>MF 6:00 - 7:50pm</t>
-  </si>
-  <si>
-    <t>MF 7:00 - 8:50pm</t>
-  </si>
-  <si>
-    <t>MF 8:00 - 9:50pm</t>
-  </si>
-  <si>
-    <t>MWF 7:00am - 8:05am</t>
-  </si>
-  <si>
-    <t>MWF 12:00pm - 1:05pm</t>
-  </si>
-  <si>
-    <t>MWF 5:00pm - 6:05pm</t>
-  </si>
-  <si>
-    <t>TR 8:00 - 9:50am</t>
-  </si>
-  <si>
-    <t>TR 10:00 - 11:50am</t>
-  </si>
-  <si>
-    <t>TR 1:00 - 2:50pm</t>
-  </si>
-  <si>
-    <t>TR 3:00 - 4:50pm</t>
-  </si>
-  <si>
-    <t>TR 5:00 - 6:50pm</t>
-  </si>
-  <si>
-    <t>TR 6:00 - 7:50pm</t>
-  </si>
-  <si>
-    <t>TR 7:00 - 8:50pm</t>
-  </si>
-  <si>
-    <t>TR 8:00 - 9:50pm</t>
-  </si>
-  <si>
-    <t>MW 7:00 - 8:15pm</t>
-  </si>
-  <si>
-    <t>MW 11:00am - 12:50pm</t>
-  </si>
-  <si>
-    <t>MF 11:00am - 12:50pm</t>
+    <t>MW 11:30 - 12:45</t>
+  </si>
+  <si>
+    <t>MW 13:00 - 14:15</t>
+  </si>
+  <si>
+    <t>MW 14:30 - 15:45</t>
+  </si>
+  <si>
+    <t>MW 16:00 - 17:15</t>
+  </si>
+  <si>
+    <t>MW 17:30 - 18:45</t>
+  </si>
+  <si>
+    <t>MW 19:00 - 20:15</t>
+  </si>
+  <si>
+    <t>MW 20:30 - 21:45</t>
+  </si>
+  <si>
+    <t>WF 11:30 - 12:45</t>
+  </si>
+  <si>
+    <t>WF 13:00 - 14:15</t>
+  </si>
+  <si>
+    <t>WF 14:30 - 15:45</t>
+  </si>
+  <si>
+    <t>WF 16:00 - 17:15</t>
+  </si>
+  <si>
+    <t>WF 17:30 - 18:45</t>
+  </si>
+  <si>
+    <t>WF 19:00 - 20:15</t>
+  </si>
+  <si>
+    <t>WF 20:30 - 21:45</t>
+  </si>
+  <si>
+    <t>MF 11:30 - 12:45</t>
+  </si>
+  <si>
+    <t>MF 13:00 - 14:15</t>
+  </si>
+  <si>
+    <t>MF 14:30 - 15:45</t>
+  </si>
+  <si>
+    <t>MF 16:00 - 17:15</t>
+  </si>
+  <si>
+    <t>MF 17:30 - 18:45</t>
+  </si>
+  <si>
+    <t>MF 19:00 - 20:15</t>
+  </si>
+  <si>
+    <t>MF 20:30 - 21:45</t>
+  </si>
+  <si>
+    <t>MWF 07:00 - 07:50</t>
+  </si>
+  <si>
+    <t>MWF 08:00 - 08:50</t>
+  </si>
+  <si>
+    <t>MWF 09:00 - 09:50</t>
+  </si>
+  <si>
+    <t>MWF 10:00 - 10:50</t>
+  </si>
+  <si>
+    <t>MWF 11:00 - 11:50</t>
+  </si>
+  <si>
+    <t>MWF 12:00 - 12:50</t>
+  </si>
+  <si>
+    <t>MWF 13:00 - 13:50</t>
+  </si>
+  <si>
+    <t>MWF 14:00 - 14:50</t>
+  </si>
+  <si>
+    <t>MWF 15:00 - 15:50</t>
+  </si>
+  <si>
+    <t>MWF 16:00 - 16:50</t>
+  </si>
+  <si>
+    <t>MWF 17:00 - 17:50</t>
+  </si>
+  <si>
+    <t>MWF 18:00 - 18:50</t>
+  </si>
+  <si>
+    <t>MWF 19:00 - 19:50</t>
+  </si>
+  <si>
+    <t>MWF 20:00 - 20:50</t>
+  </si>
+  <si>
+    <t>MWF 21:00 - 21:50</t>
+  </si>
+  <si>
+    <t>TR 07:00 - 08:15</t>
+  </si>
+  <si>
+    <t>TR 08:30 - 09:15</t>
+  </si>
+  <si>
+    <t>TR 10:00 - 11:15</t>
+  </si>
+  <si>
+    <t>TR 13:00 - 14:15</t>
+  </si>
+  <si>
+    <t>TR 14:30 - 15:45</t>
+  </si>
+  <si>
+    <t>TR 16:00 - 17:15</t>
+  </si>
+  <si>
+    <t>TR 17:30 - 18:45</t>
+  </si>
+  <si>
+    <t>TR 19:00 - 20:15</t>
+  </si>
+  <si>
+    <t>TR 20:30 - 21:45</t>
+  </si>
+  <si>
+    <t>MW 11:00 - 12:50</t>
+  </si>
+  <si>
+    <t>MW 13:00 - 14:50</t>
+  </si>
+  <si>
+    <t>MW 15:00 - 16:50</t>
+  </si>
+  <si>
+    <t>MW 17:00 - 18:50</t>
+  </si>
+  <si>
+    <t>MW 18:00 - 19:50</t>
+  </si>
+  <si>
+    <t>MW 19:00 - 20:50</t>
+  </si>
+  <si>
+    <t>MW 20:00 - 21:50</t>
+  </si>
+  <si>
+    <t>WF 11:00 - 12:50</t>
+  </si>
+  <si>
+    <t>WF 13:00 - 14:50</t>
+  </si>
+  <si>
+    <t>WF 15:00 - 16:50</t>
+  </si>
+  <si>
+    <t>WF 17:00 - 18:50</t>
+  </si>
+  <si>
+    <t>WF 18:00 - 19:50</t>
+  </si>
+  <si>
+    <t>WF 19:00 - 20:50</t>
+  </si>
+  <si>
+    <t>WF 20:00 - 21:50</t>
+  </si>
+  <si>
+    <t>MF 11:00 - 12:50</t>
+  </si>
+  <si>
+    <t>MF 13:00 - 14:50</t>
+  </si>
+  <si>
+    <t>MF 15:00 - 16:50</t>
+  </si>
+  <si>
+    <t>MF 17:00 - 18:50</t>
+  </si>
+  <si>
+    <t>MF 18:00 - 19:50</t>
+  </si>
+  <si>
+    <t>MF 19:00 - 20:50</t>
+  </si>
+  <si>
+    <t>MF 20:00 - 21:50</t>
+  </si>
+  <si>
+    <t>MWF 07:00 - 08:05</t>
+  </si>
+  <si>
+    <t>MWF 08:15 - 09:20</t>
+  </si>
+  <si>
+    <t>MWF 09:30 - 10:35</t>
+  </si>
+  <si>
+    <t>MWF 10:45 - 11:50</t>
+  </si>
+  <si>
+    <t>MWF 12:00 - 13:05</t>
+  </si>
+  <si>
+    <t>MWF 13:15 - 14:20</t>
+  </si>
+  <si>
+    <t>MWF 14:30 - 15:35</t>
+  </si>
+  <si>
+    <t>MWF 15:45 - 16:50</t>
+  </si>
+  <si>
+    <t>MWF 17:00 - 18:05</t>
+  </si>
+  <si>
+    <t>MWF 18:15 - 19:20</t>
+  </si>
+  <si>
+    <t>MWF 19:30 - 20:35</t>
+  </si>
+  <si>
+    <t>MWF 20:45 - 21:50</t>
+  </si>
+  <si>
+    <t>TR 08:00 - 09:50</t>
+  </si>
+  <si>
+    <t>TR 10:00 - 11:50</t>
+  </si>
+  <si>
+    <t>TR 13:00 - 14:50</t>
+  </si>
+  <si>
+    <t>TR 15:00 - 16:50</t>
+  </si>
+  <si>
+    <t>TR 17:00 - 18:50</t>
+  </si>
+  <si>
+    <t>TR 18:00 - 19:50</t>
+  </si>
+  <si>
+    <t>TR 19:00 - 20:50</t>
+  </si>
+  <si>
+    <t>TR 20:00 - 21:50</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -498,9 +498,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -837,16 +834,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1365,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1467,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF80D7E3-E343-414F-BE36-3299F3B3A91E}">
   <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="350" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="389" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1489,599 +1486,599 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>64</v>
+      <c r="B3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>65</v>
+      <c r="B4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>66</v>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>67</v>
+      <c r="B6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>128</v>
+      <c r="B7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
+      <c r="B8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>7</v>
+      <c r="B9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>68</v>
+      <c r="B10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>69</v>
+      <c r="B11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>70</v>
+      <c r="B12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>71</v>
+      <c r="B13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>72</v>
+      <c r="B14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
+      <c r="B15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>73</v>
+      <c r="B17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>74</v>
+      <c r="B18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>75</v>
+      <c r="B19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>76</v>
+      <c r="B20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>77</v>
+      <c r="B21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>10</v>
+      <c r="B22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>78</v>
+      <c r="B23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>79</v>
+      <c r="B24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>80</v>
+      <c r="B25" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>81</v>
+      <c r="B26" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>82</v>
+      <c r="B27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>83</v>
+      <c r="B28" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>84</v>
+      <c r="B29" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>85</v>
+      <c r="B30" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>86</v>
+      <c r="B31" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>87</v>
+      <c r="B32" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>88</v>
+      <c r="B33" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>89</v>
+      <c r="B34" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>90</v>
+      <c r="B35" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>91</v>
+      <c r="B36" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>92</v>
+      <c r="B37" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>93</v>
+      <c r="B38" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>11</v>
+      <c r="B39" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>94</v>
+      <c r="B40" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>95</v>
+      <c r="B41" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>12</v>
+      <c r="B42" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>96</v>
+      <c r="B43" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>13</v>
+      <c r="B44" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>97</v>
+      <c r="B45" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>14</v>
+      <c r="B46" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>129</v>
+      <c r="B47" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>98</v>
+      <c r="B48" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>99</v>
+      <c r="B49" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>100</v>
+      <c r="B50" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>101</v>
+      <c r="B51" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>102</v>
+      <c r="B52" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>103</v>
+      <c r="B53" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>104</v>
+      <c r="B54" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>105</v>
+      <c r="B55" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>106</v>
+      <c r="B56" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>107</v>
+      <c r="B57" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>108</v>
+      <c r="B58" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>109</v>
+      <c r="B59" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>110</v>
+      <c r="B60" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>130</v>
+      <c r="B61" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>111</v>
+      <c r="B62" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>112</v>
+      <c r="B63" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>113</v>
+      <c r="B64" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>64</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>114</v>
+      <c r="B65" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>65</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>115</v>
+      <c r="B66" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
-      <c r="B67" s="9" t="s">
-        <v>116</v>
+      <c r="B67" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>67</v>
       </c>
-      <c r="B68" s="9" t="s">
-        <v>117</v>
+      <c r="B68" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>68</v>
       </c>
-      <c r="B69" s="9" t="s">
-        <v>15</v>
+      <c r="B69" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>69</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>16</v>
+      <c r="B70" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>70</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>17</v>
+      <c r="B71" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>71</v>
       </c>
-      <c r="B72" s="9" t="s">
-        <v>118</v>
+      <c r="B72" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>72</v>
       </c>
-      <c r="B73" s="9" t="s">
-        <v>18</v>
+      <c r="B73" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>73</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>19</v>
+      <c r="B74" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>74</v>
       </c>
-      <c r="B75" s="9" t="s">
-        <v>20</v>
+      <c r="B75" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>75</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2089,88 +2086,88 @@
       <c r="A77" s="7">
         <v>76</v>
       </c>
-      <c r="B77" s="9" t="s">
-        <v>21</v>
+      <c r="B77" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>77</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>22</v>
+      <c r="B78" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>78</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>23</v>
+      <c r="B79" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>79</v>
       </c>
-      <c r="B80" s="9" t="s">
-        <v>120</v>
+      <c r="B80" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>80</v>
       </c>
-      <c r="B81" s="9" t="s">
-        <v>121</v>
+      <c r="B81" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>81</v>
       </c>
-      <c r="B82" s="9" t="s">
-        <v>122</v>
+      <c r="B82" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>82</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>123</v>
+      <c r="B83" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>124</v>
+      <c r="B84" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>84</v>
       </c>
-      <c r="B85" s="9" t="s">
-        <v>125</v>
+      <c r="B85" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>85</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>126</v>
+      <c r="B86" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>86</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>127</v>
+      <c r="B87" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2198,25 +2195,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2494,109 +2491,109 @@
   <sheetData>
     <row r="1" spans="1:35" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="U1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>